<commit_message>
Add the code - Harmful list
</commit_message>
<xml_diff>
--- a/input/EGgutPro_mircobe_list.xlsx
+++ b/input/EGgutPro_mircobe_list.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="개정이력" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="ref_개정이력" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="harmful_beneficial_taxa" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="probio_taxa" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="disease_taxa" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Output" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="이슈 정리" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="코드_이슈정리" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="harmful_taxa_old" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="beneficial_taxa_old" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="probio_old" sheetId="9" r:id="rId12"/>

</xml_diff>